<commit_message>
Add supplier, subcat and add set price
</commit_message>
<xml_diff>
--- a/Equipment Tools.xlsx
+++ b/Equipment Tools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Equipment and Tools Fields</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Category</t>
   </si>
   <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
     <t>Asset Control No.</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
     <t>UOM</t>
   </si>
   <si>
+    <t>Supplier</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date Issued </t>
   </si>
   <si>
@@ -89,6 +95,51 @@
     <t>Furniture, Fixtures and Equipment</t>
   </si>
   <si>
+    <t>Communication Equipment</t>
+  </si>
+  <si>
+    <t>FFE-COM-BCD-1002</t>
+  </si>
+  <si>
+    <t>Test DAT</t>
+  </si>
+  <si>
+    <t>sasd</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234, </t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Stephine David Severino</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>IT Department</t>
+  </si>
+  <si>
+    <t>CENPRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1001.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1001 </t>
+  </si>
+  <si>
+    <t>Computer Equipment</t>
+  </si>
+  <si>
     <t>FFE- COMP-BCD-1298</t>
   </si>
   <si>
@@ -101,19 +152,7 @@
     <t xml:space="preserve">031255648569, 012548775, </t>
   </si>
   <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>Stephine David Severino</t>
-  </si>
-  <si>
-    <t>Assigned</t>
-  </si>
-  <si>
-    <t>IT Department</t>
-  </si>
-  <si>
-    <t>CENPRI</t>
+    <t>PC REM</t>
   </si>
   <si>
     <t>Brand New</t>
@@ -122,7 +161,7 @@
     <t>350.00 PHP</t>
   </si>
   <si>
-    <t>0 PHP</t>
+    <t>700 PHP</t>
   </si>
 </sst>
 </file>
@@ -508,7 +547,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,30 +556,32 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="5.570068" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="30.563965" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="3.570557" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="15.996094" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="5.570068" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="30.563965" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="12.139893" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="28.135986" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="18.852539" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="17.852783" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="8.426514" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="10.283203" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="7.426758" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="8.426514" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="12.139893" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="18.852539" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="17.852783" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="8.426514" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="10.283203" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="7.426758" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:24">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -548,7 +589,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:24">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -615,63 +656,134 @@
       <c r="V2" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="W2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="2">
         <v>2</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="1" t="s">
+      <c r="L4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V3" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
-    <protectedRange name="p026f81593865452ef1e3b0c016311075" sqref="A3:V3" password="C724"/>
+    <protectedRange name="pe25044fc677aea1885b4f8ce2ece508b" sqref="A3:X3" password="C724"/>
+    <protectedRange name="p927dc6927eccc51dba28ca7c976cfa1a" sqref="A4:X4" password="C724"/>
   </protectedRanges>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
include get_name function  to Borrow, Encode, and Repair Controllers
</commit_message>
<xml_diff>
--- a/Equipment Tools.xlsx
+++ b/Equipment Tools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Equipment and Tools Fields</t>
   </si>
@@ -95,73 +95,97 @@
     <t>Furniture, Fixtures and Equipment</t>
   </si>
   <si>
-    <t>Communication Equipment</t>
-  </si>
-  <si>
-    <t>FFE-COM-BCD-1002</t>
-  </si>
-  <si>
-    <t>Test DAT</t>
-  </si>
-  <si>
-    <t>sasd</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234, </t>
+    <t>Office Equipment</t>
+  </si>
+  <si>
+    <t>FFE-EQU-BS-1004</t>
+  </si>
+  <si>
+    <t>2019-02-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flash Drive, 16GB </t>
+  </si>
+  <si>
+    <t>TeamGroup</t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>Stephine David Severino</t>
+    <t>2019-09-24</t>
+  </si>
+  <si>
+    <t>Julyn May Divinagracia</t>
   </si>
   <si>
     <t>Assigned</t>
   </si>
   <si>
-    <t>IT Department</t>
+    <t>Purchasing Department</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>400.00 PHP</t>
+  </si>
+  <si>
+    <t>400 PHP</t>
+  </si>
+  <si>
+    <t>Office Furnitures</t>
+  </si>
+  <si>
+    <t>FFE-COMP-BS-1138</t>
+  </si>
+  <si>
+    <t>Flash Drive, 64GB</t>
+  </si>
+  <si>
+    <t>Trascend</t>
+  </si>
+  <si>
+    <t>Mary Grace Bugna</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Warehouse Room 1</t>
   </si>
   <si>
     <t>CENPRI</t>
   </si>
   <si>
-    <t xml:space="preserve">1001.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1001 </t>
-  </si>
-  <si>
-    <t>Computer Equipment</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1298</t>
-  </si>
-  <si>
-    <t>Flashdrive 32 GB</t>
-  </si>
-  <si>
-    <t>Kingston</t>
-  </si>
-  <si>
-    <t xml:space="preserve">031255648569, 012548775, </t>
-  </si>
-  <si>
-    <t>PC REM</t>
-  </si>
-  <si>
-    <t>Brand New</t>
-  </si>
-  <si>
-    <t>350.00 PHP</t>
-  </si>
-  <si>
-    <t>700 PHP</t>
+    <t xml:space="preserve">0.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 </t>
+  </si>
+  <si>
+    <t>Flash Drive 64GB</t>
+  </si>
+  <si>
+    <t>FFE-COMP-BS-1145</t>
+  </si>
+  <si>
+    <t>Flash Drive, 16GB</t>
+  </si>
+  <si>
+    <t>Team Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFE-COMP-BS-1145, </t>
+  </si>
+  <si>
+    <t>Teranova Computers</t>
+  </si>
+  <si>
+    <t>Admin Office</t>
+  </si>
+  <si>
+    <t>357.14 PHP</t>
   </si>
 </sst>
 </file>
@@ -547,7 +571,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,29 +580,29 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="28.135986" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="19.995117" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="4.570313" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="5.570068" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="30.563965" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="5.855713" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="8.426514" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="12.139893" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="26.993408" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="18.852539" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="19.995117" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="4.570313" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="17.852783" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="8.426514" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="10.283203" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="7.426758" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="19.995117" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -673,51 +697,49 @@
       <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="2">
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="X3" s="1"/>
     </row>
@@ -726,49 +748,47 @@
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="I4" s="1"/>
       <c r="J4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="R4" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="3" t="s">
@@ -777,13 +797,80 @@
       <c r="W4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="X4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
     <protectedRange name="pe25044fc677aea1885b4f8ce2ece508b" sqref="A3:X3" password="C724"/>
     <protectedRange name="p927dc6927eccc51dba28ca7c976cfa1a" sqref="A4:X4" password="C724"/>
+    <protectedRange name="pd005e28fe538d384a15883907be295ec" sqref="A5:X5" password="C724"/>
   </protectedRanges>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>